<commit_message>
j'ai juste rajouté une 15eme modification dans le document excel
</commit_message>
<xml_diff>
--- a/Audit-SEO.xlsx
+++ b/Audit-SEO.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="51">
   <si>
     <t>Catégorie</t>
   </si>
@@ -171,6 +171,15 @@
   </si>
   <si>
     <t>Rende le focus visible en définissant les règles css nécessaires</t>
+  </si>
+  <si>
+    <t>Répéter les mêmes mots clés est une pratique pénalisé par Google</t>
+  </si>
+  <si>
+    <t>Modifier les mots clés répétés par des mots clés pertinants</t>
+  </si>
+  <si>
+    <t>balise meta keywords à modifier + supprimer les balises méta keywords ittérées dans la page html</t>
   </si>
 </sst>
 </file>
@@ -493,8 +502,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.26953125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -742,6 +751,18 @@
       <c r="E14" s="2"/>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>49</v>
+      </c>
       <c r="E15" s="2"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
quelques modification ont été faite dans le fichier excel et j'ai mis le site avant modifications sur le dossier principal
</commit_message>
<xml_diff>
--- a/Audit-SEO.xlsx
+++ b/Audit-SEO.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="54">
   <si>
     <t>Catégorie</t>
   </si>
@@ -59,60 +59,33 @@
     <t>accessibilité</t>
   </si>
   <si>
-    <t>Créer des liens vers des annuaires est une mauvaise pratique pénéalisé par google car cela augmente le nombre de lien à crawler</t>
-  </si>
-  <si>
-    <t>performance + accessibilité</t>
-  </si>
-  <si>
     <t>performance</t>
   </si>
   <si>
     <t>L'atribut des images et des liens sont identiques au lieu d'être personnalisés</t>
   </si>
   <si>
-    <t>Diriger plusieurs fois l'utilisateur vers le même lien est une pratique pénalisé par google car, on répéte le même contenu. Cela à aussi pour effet de perturber l'utilisateur car le site n'est pas structuré correctement</t>
-  </si>
-  <si>
-    <t>Mettre du contenu textuel sous forme d'image empêche non seulement aux utilisateurs d'ajuster la taille du texte et la mise en gras mais aussi rajoute du poid au document via la taille des img donc nuit niveau performance</t>
-  </si>
-  <si>
     <t>Laisser un format d'image plus important que la taille du contenant n'est pas utile puisque celle-çi peut être redimensionné pour alléger le poid du site et donc sa performance</t>
   </si>
   <si>
     <t>Les liens vers des annuaires dans le footer</t>
   </si>
   <si>
-    <t>Trop de liens vont vers la page 2 "contact"+ lien acceuil dans page d'acceuil + le logo allant vers l'acceuil</t>
-  </si>
-  <si>
     <t>Citations + 2 titres en img au lieu d'être écrit dans des balises p,h2</t>
   </si>
   <si>
-    <t>Format d'images plus importants que leurs contenants</t>
-  </si>
-  <si>
-    <t>Paramétrer lang="fr-fr"  dans html</t>
-  </si>
-  <si>
     <t>Personnaliser alt en fonction du lien ou du contenu de l'image</t>
   </si>
   <si>
     <t>Préférer des liens de qualités comme les réseaux sociaux ou les partenaires et éviter tous ce qui est annuaires</t>
   </si>
   <si>
-    <t>Préférer une bonne structuration sans répéter plusieurs fois le même contenu</t>
-  </si>
-  <si>
     <t>Changer les images contenant du texte par des balises &lt;p&gt;,&lt;h2&gt;</t>
   </si>
   <si>
     <t>Fichiers HTLM, CSS, JASCRIPT trops lourds</t>
   </si>
   <si>
-    <t>Laisser des fichiers lourds tels que html, css javascript ect sans réduire leur taille réduit les performance du site concerné</t>
-  </si>
-  <si>
     <t>Réduire le format d'image au format adapté au contenant tout en pensant au responsive et à la résolution maximum nécessaire.</t>
   </si>
   <si>
@@ -179,14 +152,102 @@
     <t>Modifier les mots clés répétés par des mots clés pertinants</t>
   </si>
   <si>
-    <t>balise meta keywords à modifier + supprimer les balises méta keywords ittérées dans la page html</t>
+    <t>Paramétrer lang="fr"  dans html</t>
+  </si>
+  <si>
+    <r>
+      <t>Créer des liens vers des annuaires est une mauvaise pratique pénéalisé par google car cela augmente le nombre de lien à crawler.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Considéré comme une pratique blackhat/ liens non pertinens</t>
+    </r>
+  </si>
+  <si>
+    <t>partenaires non pertinents.</t>
+  </si>
+  <si>
+    <t>peut être blackhat</t>
+  </si>
+  <si>
+    <t>à enlever</t>
+  </si>
+  <si>
+    <t>texte</t>
+  </si>
+  <si>
+    <t>à revoir</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Mettre du contenu textuel sous forme d'image empêche non seulement aux utilisateurs d'ajuster la taille du texte et la mise en gras mais aussi </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">rajoute du poid au document via la taille des img donc nuit niveau </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>performance</t>
+    </r>
+  </si>
+  <si>
+    <t>texte à supprimer</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">resolution et </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>format</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> d'images plus importants que leurs contenants</t>
+    </r>
+  </si>
+  <si>
+    <t>balise meta keywords à modifier + supprimer lesdiv class keywords ittérées dans la page html</t>
+  </si>
+  <si>
+    <t>Appeler des fichiers lourds tels que html, css javascript ect sans réduire leur taille réduit les performance du site concerné</t>
+  </si>
+  <si>
+    <t>liens acceuil +page 2 problème responsive dans la page 2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -223,8 +284,21 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -235,6 +309,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF7030A0"/>
         <bgColor rgb="FF7030A0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -257,7 +337,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -285,6 +365,19 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -503,7 +596,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.26953125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -565,26 +658,26 @@
         <v>6</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="E2" s="10"/>
       <c r="F2" s="9"/>
     </row>
     <row r="3" spans="1:26" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="E3" s="10"/>
       <c r="F3" s="9"/>
@@ -594,129 +687,123 @@
         <v>7</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="E4" s="10"/>
       <c r="F4" s="9"/>
     </row>
-    <row r="5" spans="1:26" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>24</v>
-      </c>
+    <row r="5" spans="1:26" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A5" s="13"/>
+      <c r="B5" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
       <c r="E5" s="10"/>
       <c r="F5" s="9"/>
     </row>
-    <row r="6" spans="1:26" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>11</v>
+    <row r="6" spans="1:26" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
+        <v>9</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="E6" s="10"/>
       <c r="F6" s="9"/>
     </row>
     <row r="7" spans="1:26" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>16</v>
-      </c>
       <c r="D7" s="6" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="E7" s="10"/>
       <c r="F7" s="9"/>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="3"/>
     </row>
     <row r="9" spans="1:26" ht="45" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="E9" s="2"/>
     </row>
     <row r="10" spans="1:26" ht="45" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:26" ht="30" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="6" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="E12" s="2"/>
     </row>
@@ -725,13 +812,13 @@
         <v>9</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="E13" s="2"/>
     </row>
@@ -740,13 +827,13 @@
         <v>9</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="E14" s="2"/>
     </row>
@@ -755,33 +842,62 @@
         <v>7</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="15"/>
+      <c r="B19" s="11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>